<commit_message>
adjusting notebook for streamlit
</commit_message>
<xml_diff>
--- a/mi_2021_oor_data.xlsx
+++ b/mi_2021_oor_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narainyucel/Google Drive/MADS/community_corps/CHN/CHN analysis/CC_Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45A51876-737C-9241-B928-FEAD857FA758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94694ED-F3B4-9348-AAA2-A49769992871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41420" yWindow="2360" windowWidth="23260" windowHeight="12580" xr2:uid="{B848C4AF-73ED-4619-ADCB-795B5E697368}"/>
+    <workbookView xWindow="29040" yWindow="500" windowWidth="19420" windowHeight="12580" activeTab="2" xr2:uid="{B848C4AF-73ED-4619-ADCB-795B5E697368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1466,15 +1466,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1795,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E77F240-49D5-4587-BD5B-C4D608B181B0}">
   <dimension ref="A1:AV105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -17802,7 +17802,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1296A14B-B3C6-4AD5-AF89-86A8E50CD642}">
   <dimension ref="A1:IV79"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
@@ -18670,8 +18670,8 @@
         <v>1060.8098760796599</v>
       </c>
       <c r="D8" s="41"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
       <c r="H8" s="42"/>
     </row>
     <row r="9" spans="1:256" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -18683,8 +18683,8 @@
         <v>1294.72729728488</v>
       </c>
       <c r="D9" s="41"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
       <c r="H9" s="42"/>
     </row>
     <row r="10" spans="1:256" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -18696,8 +18696,8 @@
         <v>1713.1379444167201</v>
       </c>
       <c r="D10" s="41"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
       <c r="H10" s="42"/>
     </row>
     <row r="11" spans="1:256" s="33" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -18709,8 +18709,8 @@
         <v>1987.93296558202</v>
       </c>
       <c r="D11" s="41"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
       <c r="H11" s="42"/>
     </row>
     <row r="12" spans="1:256" s="33" customFormat="1" x14ac:dyDescent="0.15">
@@ -19065,10 +19065,10 @@
         <f>C32/40</f>
         <v>2.5339943421270998</v>
       </c>
-      <c r="E39" s="80" t="s">
+      <c r="E39" s="82" t="s">
         <v>270</v>
       </c>
-      <c r="F39" s="80" t="s">
+      <c r="F39" s="82" t="s">
         <v>271</v>
       </c>
     </row>
@@ -19080,8 +19080,8 @@
         <f>C33/40</f>
         <v>2.8138192999460498</v>
       </c>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
     </row>
     <row r="41" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="B41" s="30" t="s">
@@ -19091,8 +19091,8 @@
         <f>C34/40</f>
         <v>3.4342899132225</v>
       </c>
-      <c r="E41" s="80"/>
-      <c r="F41" s="80"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="82"/>
     </row>
     <row r="42" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="B42" s="30" t="s">
@@ -19102,8 +19102,8 @@
         <f>C35/40</f>
         <v>4.5441324785589501</v>
       </c>
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
     </row>
     <row r="43" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="B43" s="30" t="s">
@@ -19113,8 +19113,8 @@
         <f>C36/40</f>
         <v>5.2730317389443497</v>
       </c>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="82"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44" s="29" t="s">
@@ -19912,8 +19912,8 @@
         <v>1024.9608763082899</v>
       </c>
       <c r="D67" s="41"/>
-      <c r="E67" s="78"/>
-      <c r="F67" s="78"/>
+      <c r="E67" s="80"/>
+      <c r="F67" s="80"/>
       <c r="G67" s="48"/>
       <c r="H67" s="49"/>
       <c r="I67" s="50"/>
@@ -20174,8 +20174,8 @@
         <v>1639.9374020932701</v>
       </c>
       <c r="D68" s="41"/>
-      <c r="E68" s="78"/>
-      <c r="F68" s="78"/>
+      <c r="E68" s="80"/>
+      <c r="F68" s="80"/>
       <c r="G68" s="52"/>
       <c r="H68" s="49"/>
       <c r="I68" s="50"/>
@@ -20436,8 +20436,8 @@
         <v>2049.9217526165899</v>
       </c>
       <c r="D69" s="41"/>
-      <c r="E69" s="79"/>
-      <c r="F69" s="79"/>
+      <c r="E69" s="81"/>
+      <c r="F69" s="81"/>
       <c r="G69" s="48"/>
       <c r="H69" s="49"/>
       <c r="I69" s="50"/>
@@ -22545,13 +22545,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E19:E23"/>
-    <mergeCell ref="F19:F23"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E13:E17"/>
-    <mergeCell ref="F13:F17"/>
     <mergeCell ref="E56:E60"/>
     <mergeCell ref="F56:F60"/>
     <mergeCell ref="E66:E69"/>
@@ -22562,6 +22555,13 @@
     <mergeCell ref="F39:F43"/>
     <mergeCell ref="E49:E53"/>
     <mergeCell ref="F49:F53"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="F19:F23"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="F13:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>